<commit_message>
Fix for FHIR-30635 - Update Benefit Payment Status slice name ,cardinality and must support
</commit_message>
<xml_diff>
--- a/input/images/CARINProfileComparison.xlsx
+++ b/input/images/CARINProfileComparison.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10913"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23530"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/skravitz/git/carin-bb/fsh/ig-data/input/images/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Dev\FHIR\FSH\DaVinciIG_Dev\CARINBB\carin-bb\input\images\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F783744-8C00-3442-9382-5896696A5F38}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AED0C62F-8A38-4EC7-A9F4-610C818F2F9C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="13860" yWindow="520" windowWidth="38720" windowHeight="24740" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-2025" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="EOBProfileComparison" sheetId="1" r:id="rId1"/>
@@ -276,9 +276,6 @@
     <t>slice: adjudicationamounttype</t>
   </si>
   <si>
-    <t>slice: inoutnetwork</t>
-  </si>
-  <si>
     <t>slice: allowedUnits</t>
   </si>
   <si>
@@ -503,13 +500,16 @@
   </si>
   <si>
     <t>updated</t>
+  </si>
+  <si>
+    <t>slice: benefitpaymentstatus</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="11" x14ac:knownFonts="1">
+  <fonts count="11">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -1193,6 +1193,74 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="9" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="9" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="9" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="9" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="9" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="9" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="9" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="10" fillId="0" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="9" fillId="13" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="2" fillId="6" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1253,74 +1321,6 @@
     <xf numFmtId="49" fontId="2" fillId="4" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="0" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="9" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="9" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="9" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="9" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="9" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="9" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="9" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="10" fillId="0" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="9" fillId="13" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1711,25 +1711,25 @@
   </sheetPr>
   <dimension ref="A1:K51"/>
   <sheetViews>
-    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A12" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="L18" sqref="L18"/>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A21" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B48" sqref="B48"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="24" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="23.25"/>
   <cols>
     <col min="1" max="1" width="24" style="6" customWidth="1"/>
-    <col min="2" max="2" width="35.6640625" style="2" customWidth="1"/>
-    <col min="3" max="3" width="11.33203125" style="120" customWidth="1"/>
+    <col min="2" max="2" width="35.625" style="2" customWidth="1"/>
+    <col min="3" max="3" width="11.375" style="100" customWidth="1"/>
     <col min="4" max="4" width="32" style="2" customWidth="1"/>
-    <col min="5" max="5" width="38.6640625" style="2" customWidth="1"/>
-    <col min="6" max="6" width="36.1640625" style="2" customWidth="1"/>
-    <col min="7" max="7" width="46.33203125" style="2" customWidth="1"/>
-    <col min="8" max="8" width="45.1640625" style="2" customWidth="1"/>
-    <col min="9" max="16384" width="10.83203125" style="1"/>
+    <col min="5" max="5" width="38.625" style="2" customWidth="1"/>
+    <col min="6" max="6" width="36.125" style="2" customWidth="1"/>
+    <col min="7" max="7" width="46.375" style="2" customWidth="1"/>
+    <col min="8" max="8" width="45.125" style="2" customWidth="1"/>
+    <col min="9" max="16384" width="10.875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" s="3" customFormat="1" ht="25" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" s="3" customFormat="1">
       <c r="A1" s="17" t="s">
         <v>1</v>
       </c>
@@ -1737,7 +1737,7 @@
         <v>5</v>
       </c>
       <c r="C1" s="18" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D1" s="18" t="s">
         <v>25</v>
@@ -1755,25 +1755,25 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:11" s="3" customFormat="1" ht="36" x14ac:dyDescent="0.3">
-      <c r="A2" s="122" t="s">
+    <row r="2" spans="1:11" s="3" customFormat="1" ht="32.25">
+      <c r="A2" s="102" t="s">
+        <v>143</v>
+      </c>
+      <c r="B2" s="83" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" s="84" t="s">
+        <v>112</v>
+      </c>
+      <c r="D2" s="101" t="s">
         <v>144</v>
       </c>
-      <c r="B2" s="103" t="s">
-        <v>6</v>
-      </c>
-      <c r="C2" s="104" t="s">
-        <v>113</v>
-      </c>
-      <c r="D2" s="121" t="s">
-        <v>145</v>
-      </c>
-      <c r="E2" s="101"/>
-      <c r="F2" s="101"/>
-      <c r="G2" s="101"/>
-      <c r="H2" s="102"/>
-    </row>
-    <row r="3" spans="1:11" s="3" customFormat="1" ht="54" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="E2" s="81"/>
+      <c r="F2" s="81"/>
+      <c r="G2" s="81"/>
+      <c r="H2" s="82"/>
+    </row>
+    <row r="3" spans="1:11" s="3" customFormat="1" ht="49.5" thickBot="1">
       <c r="A3" s="24" t="s">
         <v>6</v>
       </c>
@@ -1796,26 +1796,26 @@
       </c>
       <c r="K3" s="5"/>
     </row>
-    <row r="4" spans="1:11" s="3" customFormat="1" ht="36" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="88" t="s">
-        <v>84</v>
+    <row r="4" spans="1:11" s="3" customFormat="1" ht="36" customHeight="1">
+      <c r="A4" s="112" t="s">
+        <v>83</v>
       </c>
       <c r="B4" s="29" t="s">
         <v>43</v>
       </c>
-      <c r="C4" s="105" t="s">
-        <v>113</v>
+      <c r="C4" s="85" t="s">
+        <v>112</v>
       </c>
       <c r="D4" s="30" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="E4" s="30"/>
       <c r="F4" s="30"/>
       <c r="G4" s="30"/>
       <c r="H4" s="31"/>
     </row>
-    <row r="5" spans="1:11" s="3" customFormat="1" ht="25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="89"/>
+    <row r="5" spans="1:11" s="3" customFormat="1" ht="24" thickBot="1">
+      <c r="A5" s="113"/>
       <c r="B5" s="26"/>
       <c r="C5" s="27"/>
       <c r="D5" s="26"/>
@@ -1824,68 +1824,68 @@
       <c r="G5" s="26"/>
       <c r="H5" s="32"/>
     </row>
-    <row r="6" spans="1:11" ht="34" x14ac:dyDescent="0.2">
-      <c r="A6" s="91" t="s">
+    <row r="6" spans="1:11" ht="31.5">
+      <c r="A6" s="115" t="s">
         <v>7</v>
       </c>
       <c r="B6" s="30" t="s">
         <v>6</v>
       </c>
-      <c r="C6" s="105"/>
+      <c r="C6" s="85"/>
       <c r="D6" s="30"/>
       <c r="E6" s="30" t="s">
+        <v>116</v>
+      </c>
+      <c r="F6" s="30" t="s">
         <v>117</v>
       </c>
-      <c r="F6" s="30" t="s">
+      <c r="G6" s="30" t="s">
         <v>118</v>
       </c>
-      <c r="G6" s="30" t="s">
-        <v>119</v>
-      </c>
       <c r="H6" s="31"/>
     </row>
-    <row r="7" spans="1:11" ht="24" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="92"/>
+    <row r="7" spans="1:11" ht="24" customHeight="1">
+      <c r="A7" s="116"/>
       <c r="B7" s="16" t="s">
         <v>7</v>
       </c>
-      <c r="C7" s="106"/>
+      <c r="C7" s="86"/>
       <c r="D7" s="16"/>
       <c r="E7" s="16" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="F7" s="16" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="G7" s="16" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="H7" s="20"/>
     </row>
-    <row r="8" spans="1:11" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="93"/>
+    <row r="8" spans="1:11" ht="24" customHeight="1" thickBot="1">
+      <c r="A8" s="117"/>
       <c r="B8" s="22" t="s">
         <v>8</v>
       </c>
-      <c r="C8" s="107" t="s">
+      <c r="C8" s="87" t="s">
         <v>24</v>
       </c>
       <c r="D8" s="22"/>
       <c r="E8" s="22" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="F8" s="22"/>
       <c r="G8" s="22"/>
       <c r="H8" s="23"/>
     </row>
-    <row r="9" spans="1:11" ht="26" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11" ht="24" thickBot="1">
       <c r="A9" s="33" t="s">
         <v>38</v>
       </c>
       <c r="B9" s="34" t="s">
         <v>39</v>
       </c>
-      <c r="C9" s="108"/>
+      <c r="C9" s="88"/>
       <c r="D9" s="34" t="s">
         <v>40</v>
       </c>
@@ -1894,42 +1894,42 @@
       <c r="G9" s="35"/>
       <c r="H9" s="36"/>
     </row>
-    <row r="10" spans="1:11" ht="24" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="94" t="s">
+    <row r="10" spans="1:11" ht="24" customHeight="1">
+      <c r="A10" s="118" t="s">
         <v>11</v>
       </c>
       <c r="B10" s="37" t="s">
         <v>11</v>
       </c>
-      <c r="C10" s="105"/>
+      <c r="C10" s="85"/>
       <c r="D10" s="38"/>
       <c r="E10" s="38" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="F10" s="38"/>
       <c r="G10" s="38"/>
       <c r="H10" s="39"/>
     </row>
-    <row r="11" spans="1:11" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="95"/>
+    <row r="11" spans="1:11" ht="24" customHeight="1" thickBot="1">
+      <c r="A11" s="119"/>
       <c r="B11" s="40" t="s">
         <v>6</v>
       </c>
       <c r="C11" s="27"/>
       <c r="D11" s="41"/>
       <c r="E11" s="41" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="F11" s="41"/>
       <c r="G11" s="41"/>
       <c r="H11" s="42"/>
     </row>
-    <row r="12" spans="1:11" ht="26" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:11" ht="24" thickBot="1">
       <c r="A12" s="43" t="s">
         <v>36</v>
       </c>
       <c r="B12" s="44"/>
-      <c r="C12" s="109"/>
+      <c r="C12" s="89"/>
       <c r="D12" s="44" t="s">
         <v>37</v>
       </c>
@@ -1938,14 +1938,14 @@
       <c r="G12" s="45"/>
       <c r="H12" s="46"/>
     </row>
-    <row r="13" spans="1:11" ht="51" x14ac:dyDescent="0.2">
-      <c r="A13" s="88" t="s">
+    <row r="13" spans="1:11" ht="47.25">
+      <c r="A13" s="112" t="s">
         <v>12</v>
       </c>
       <c r="B13" s="47" t="s">
         <v>13</v>
       </c>
-      <c r="C13" s="110"/>
+      <c r="C13" s="90"/>
       <c r="D13" s="47" t="s">
         <v>75</v>
       </c>
@@ -1954,50 +1954,50 @@
       <c r="G13" s="48"/>
       <c r="H13" s="49"/>
     </row>
-    <row r="14" spans="1:11" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="89"/>
+    <row r="14" spans="1:11" ht="24" customHeight="1" thickBot="1">
+      <c r="A14" s="113"/>
       <c r="B14" s="22" t="s">
         <v>6</v>
       </c>
-      <c r="C14" s="107" t="s">
-        <v>113</v>
+      <c r="C14" s="87" t="s">
+        <v>112</v>
       </c>
       <c r="D14" s="22" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="E14" s="50"/>
       <c r="F14" s="50"/>
       <c r="G14" s="50"/>
       <c r="H14" s="51"/>
     </row>
-    <row r="15" spans="1:11" ht="34" x14ac:dyDescent="0.2">
-      <c r="A15" s="96" t="s">
+    <row r="15" spans="1:11" ht="15.75">
+      <c r="A15" s="120" t="s">
         <v>10</v>
       </c>
       <c r="B15" s="47" t="s">
         <v>17</v>
       </c>
-      <c r="C15" s="110"/>
+      <c r="C15" s="90"/>
       <c r="D15" s="47"/>
       <c r="E15" s="47" t="s">
+        <v>119</v>
+      </c>
+      <c r="F15" s="47" t="s">
+        <v>119</v>
+      </c>
+      <c r="G15" s="47" t="s">
         <v>120</v>
       </c>
-      <c r="F15" s="47" t="s">
-        <v>120</v>
-      </c>
-      <c r="G15" s="47" t="s">
+      <c r="H15" s="52" t="s">
         <v>121</v>
       </c>
-      <c r="H15" s="52" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="16" spans="1:11" ht="49" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="97"/>
+    </row>
+    <row r="16" spans="1:11" ht="48.95" customHeight="1">
+      <c r="A16" s="121"/>
       <c r="B16" s="57" t="s">
         <v>58</v>
       </c>
-      <c r="C16" s="111"/>
+      <c r="C16" s="91"/>
       <c r="D16" s="57" t="s">
         <v>74</v>
       </c>
@@ -2014,28 +2014,28 @@
         <v>20</v>
       </c>
     </row>
-    <row r="17" spans="1:8" ht="69" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="98"/>
+    <row r="17" spans="1:8" ht="63.75" thickBot="1">
+      <c r="A17" s="122"/>
       <c r="B17" s="59" t="s">
-        <v>83</v>
-      </c>
-      <c r="C17" s="112" t="s">
-        <v>93</v>
+        <v>82</v>
+      </c>
+      <c r="C17" s="92" t="s">
+        <v>92</v>
       </c>
       <c r="D17" s="59"/>
       <c r="E17" s="59"/>
       <c r="F17" s="59"/>
       <c r="G17" s="59" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="H17" s="60"/>
     </row>
-    <row r="18" spans="1:8" ht="40" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:8" ht="39.950000000000003" customHeight="1" thickBot="1">
       <c r="A18" s="53" t="s">
         <v>9</v>
       </c>
       <c r="B18" s="61"/>
-      <c r="C18" s="113"/>
+      <c r="C18" s="93"/>
       <c r="D18" s="61" t="s">
         <v>74</v>
       </c>
@@ -2048,68 +2048,68 @@
       <c r="G18" s="62"/>
       <c r="H18" s="63"/>
     </row>
-    <row r="19" spans="1:8" ht="40" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="81" t="s">
+    <row r="19" spans="1:8" ht="39.950000000000003" customHeight="1" thickBot="1">
+      <c r="A19" s="105" t="s">
         <v>60</v>
       </c>
       <c r="B19" s="73" t="s">
+        <v>138</v>
+      </c>
+      <c r="C19" s="94" t="s">
+        <v>112</v>
+      </c>
+      <c r="D19" s="80" t="s">
         <v>139</v>
-      </c>
-      <c r="C19" s="114" t="s">
-        <v>113</v>
-      </c>
-      <c r="D19" s="80" t="s">
-        <v>140</v>
       </c>
       <c r="E19" s="73"/>
       <c r="F19" s="73"/>
       <c r="G19" s="78"/>
       <c r="H19" s="79"/>
     </row>
-    <row r="20" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="90"/>
+    <row r="20" spans="1:8" ht="30" customHeight="1">
+      <c r="A20" s="114"/>
       <c r="B20" s="64" t="s">
         <v>27</v>
       </c>
-      <c r="C20" s="115" t="s">
-        <v>113</v>
+      <c r="C20" s="95" t="s">
+        <v>112</v>
       </c>
       <c r="D20" s="64"/>
       <c r="E20" s="64" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="F20" s="64" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="G20" s="64" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="H20" s="65" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="21" spans="1:8" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="90"/>
+        <v>113</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" ht="17.100000000000001" customHeight="1">
+      <c r="A21" s="114"/>
       <c r="B21" s="57" t="s">
         <v>28</v>
       </c>
-      <c r="C21" s="111" t="s">
-        <v>113</v>
+      <c r="C21" s="91" t="s">
+        <v>112</v>
       </c>
       <c r="D21" s="57"/>
       <c r="E21" s="57"/>
       <c r="F21" s="57"/>
       <c r="G21" s="57" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="H21" s="58"/>
     </row>
-    <row r="22" spans="1:8" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="90"/>
+    <row r="22" spans="1:8" ht="17.100000000000001" customHeight="1">
+      <c r="A22" s="114"/>
       <c r="B22" s="66" t="s">
-        <v>124</v>
-      </c>
-      <c r="C22" s="116"/>
+        <v>123</v>
+      </c>
+      <c r="C22" s="96"/>
       <c r="D22" s="66"/>
       <c r="E22" s="66" t="s">
         <v>2</v>
@@ -2124,100 +2124,100 @@
         <v>2</v>
       </c>
     </row>
-    <row r="23" spans="1:8" ht="34" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="90"/>
+    <row r="23" spans="1:8" ht="33.950000000000003" customHeight="1">
+      <c r="A23" s="114"/>
       <c r="B23" s="57" t="s">
         <v>29</v>
       </c>
-      <c r="C23" s="111" t="s">
+      <c r="C23" s="91" t="s">
         <v>24</v>
       </c>
       <c r="D23" s="57"/>
       <c r="E23" s="57" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="F23" s="57" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="G23" s="57"/>
       <c r="H23" s="58"/>
     </row>
-    <row r="24" spans="1:8" ht="31" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="90"/>
+    <row r="24" spans="1:8" ht="30.95" customHeight="1">
+      <c r="A24" s="114"/>
       <c r="B24" s="66" t="s">
         <v>30</v>
       </c>
-      <c r="C24" s="116" t="s">
+      <c r="C24" s="96" t="s">
         <v>24</v>
       </c>
       <c r="D24" s="66"/>
       <c r="E24" s="66" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="F24" s="66" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="G24" s="66"/>
       <c r="H24" s="67"/>
     </row>
-    <row r="25" spans="1:8" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="90"/>
+    <row r="25" spans="1:8" ht="17.100000000000001" customHeight="1">
+      <c r="A25" s="114"/>
       <c r="B25" s="57" t="s">
         <v>31</v>
       </c>
-      <c r="C25" s="111" t="s">
+      <c r="C25" s="91" t="s">
         <v>24</v>
       </c>
       <c r="D25" s="57"/>
       <c r="E25" s="57" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="F25" s="57" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="G25" s="57"/>
       <c r="H25" s="58"/>
     </row>
-    <row r="26" spans="1:8" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A26" s="90"/>
+    <row r="26" spans="1:8" ht="17.100000000000001" customHeight="1">
+      <c r="A26" s="114"/>
       <c r="B26" s="66" t="s">
         <v>32</v>
       </c>
-      <c r="C26" s="116" t="s">
+      <c r="C26" s="96" t="s">
         <v>24</v>
       </c>
       <c r="D26" s="66"/>
       <c r="E26" s="66" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="F26" s="66" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="G26" s="66"/>
       <c r="H26" s="67"/>
     </row>
-    <row r="27" spans="1:8" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A27" s="90"/>
+    <row r="27" spans="1:8" ht="17.100000000000001" customHeight="1">
+      <c r="A27" s="114"/>
       <c r="B27" s="57" t="s">
         <v>68</v>
       </c>
-      <c r="C27" s="111" t="s">
-        <v>142</v>
+      <c r="C27" s="91" t="s">
+        <v>141</v>
       </c>
       <c r="D27" s="57"/>
       <c r="E27" s="57" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="F27" s="57"/>
       <c r="G27" s="57"/>
       <c r="H27" s="58"/>
     </row>
-    <row r="28" spans="1:8" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A28" s="90"/>
+    <row r="28" spans="1:8" ht="17.100000000000001" customHeight="1">
+      <c r="A28" s="114"/>
       <c r="B28" s="66" t="s">
         <v>33</v>
       </c>
-      <c r="C28" s="116" t="s">
+      <c r="C28" s="96" t="s">
         <v>23</v>
       </c>
       <c r="D28" s="66"/>
@@ -2228,12 +2228,12 @@
         <v>65</v>
       </c>
     </row>
-    <row r="29" spans="1:8" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A29" s="90"/>
+    <row r="29" spans="1:8" ht="17.100000000000001" customHeight="1">
+      <c r="A29" s="114"/>
       <c r="B29" s="57" t="s">
-        <v>126</v>
-      </c>
-      <c r="C29" s="111" t="s">
+        <v>125</v>
+      </c>
+      <c r="C29" s="91" t="s">
         <v>23</v>
       </c>
       <c r="D29" s="57"/>
@@ -2244,12 +2244,12 @@
         <v>66</v>
       </c>
     </row>
-    <row r="30" spans="1:8" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A30" s="90"/>
+    <row r="30" spans="1:8" ht="17.100000000000001" customHeight="1">
+      <c r="A30" s="114"/>
       <c r="B30" s="66" t="s">
-        <v>127</v>
-      </c>
-      <c r="C30" s="116"/>
+        <v>126</v>
+      </c>
+      <c r="C30" s="96"/>
       <c r="D30" s="66"/>
       <c r="E30" s="66"/>
       <c r="F30" s="66"/>
@@ -2258,12 +2258,12 @@
         <v>3</v>
       </c>
     </row>
-    <row r="31" spans="1:8" ht="19" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A31" s="90"/>
+    <row r="31" spans="1:8" ht="18.95" customHeight="1">
+      <c r="A31" s="114"/>
       <c r="B31" s="57" t="s">
-        <v>101</v>
-      </c>
-      <c r="C31" s="111" t="s">
+        <v>100</v>
+      </c>
+      <c r="C31" s="91" t="s">
         <v>23</v>
       </c>
       <c r="D31" s="57"/>
@@ -2271,15 +2271,15 @@
       <c r="F31" s="57"/>
       <c r="G31" s="57"/>
       <c r="H31" s="58" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="32" spans="1:8" ht="33" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A32" s="90"/>
+        <v>101</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" ht="33" customHeight="1">
+      <c r="A32" s="114"/>
       <c r="B32" s="66" t="s">
         <v>34</v>
       </c>
-      <c r="C32" s="116" t="s">
+      <c r="C32" s="96" t="s">
         <v>23</v>
       </c>
       <c r="D32" s="66"/>
@@ -2287,15 +2287,15 @@
       <c r="F32" s="66"/>
       <c r="G32" s="66"/>
       <c r="H32" s="67" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="33" spans="1:8" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A33" s="90"/>
+        <v>99</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" ht="17.100000000000001" customHeight="1">
+      <c r="A33" s="114"/>
       <c r="B33" s="57" t="s">
         <v>35</v>
       </c>
-      <c r="C33" s="111"/>
+      <c r="C33" s="91"/>
       <c r="D33" s="57"/>
       <c r="E33" s="57"/>
       <c r="F33" s="57"/>
@@ -2304,198 +2304,198 @@
         <v>3</v>
       </c>
     </row>
-    <row r="34" spans="1:8" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A34" s="90"/>
+    <row r="34" spans="1:8" ht="17.100000000000001" customHeight="1">
+      <c r="A34" s="114"/>
       <c r="B34" s="66" t="s">
-        <v>80</v>
-      </c>
-      <c r="C34" s="116"/>
+        <v>79</v>
+      </c>
+      <c r="C34" s="96"/>
       <c r="D34" s="66"/>
       <c r="E34" s="66" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="F34" s="66"/>
       <c r="G34" s="66"/>
       <c r="H34" s="67"/>
     </row>
-    <row r="35" spans="1:8" ht="17" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="82"/>
+    <row r="35" spans="1:8" ht="17.100000000000001" customHeight="1" thickBot="1">
+      <c r="A35" s="106"/>
       <c r="B35" s="68" t="s">
-        <v>81</v>
-      </c>
-      <c r="C35" s="117"/>
+        <v>80</v>
+      </c>
+      <c r="C35" s="97"/>
       <c r="D35" s="68"/>
       <c r="E35" s="68"/>
       <c r="F35" s="68"/>
       <c r="G35" s="68" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="H35" s="69"/>
     </row>
-    <row r="36" spans="1:8" ht="26" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:8" ht="24" thickBot="1">
       <c r="A36" s="54" t="s">
         <v>61</v>
       </c>
       <c r="B36" s="70" t="s">
         <v>6</v>
       </c>
-      <c r="C36" s="118" t="s">
-        <v>113</v>
+      <c r="C36" s="98" t="s">
+        <v>112</v>
       </c>
       <c r="D36" s="70" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="E36" s="70"/>
       <c r="F36" s="70"/>
       <c r="G36" s="71"/>
       <c r="H36" s="72"/>
     </row>
-    <row r="37" spans="1:8" ht="34" x14ac:dyDescent="0.2">
-      <c r="A37" s="99" t="s">
+    <row r="37" spans="1:8" ht="31.5">
+      <c r="A37" s="123" t="s">
         <v>62</v>
       </c>
       <c r="B37" s="73" t="s">
         <v>77</v>
       </c>
-      <c r="C37" s="114"/>
+      <c r="C37" s="94"/>
       <c r="D37" s="73"/>
       <c r="E37" s="73" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="F37" s="73" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="G37" s="73" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="H37" s="74" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="38" spans="1:8" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="100"/>
+        <v>109</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8" ht="24" customHeight="1" thickBot="1">
+      <c r="A38" s="124"/>
       <c r="B38" s="59" t="s">
-        <v>78</v>
-      </c>
-      <c r="C38" s="112" t="s">
-        <v>113</v>
+        <v>152</v>
+      </c>
+      <c r="C38" s="92" t="s">
+        <v>112</v>
       </c>
       <c r="D38" s="59"/>
       <c r="E38" s="59" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="F38" s="59" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="G38" s="59"/>
       <c r="H38" s="60" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="39" spans="1:8" ht="52" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A39" s="81" t="s">
-        <v>138</v>
+        <v>111</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8" ht="51.95" customHeight="1">
+      <c r="A39" s="105" t="s">
+        <v>137</v>
       </c>
       <c r="B39" s="73" t="s">
-        <v>128</v>
-      </c>
-      <c r="C39" s="114" t="s">
-        <v>106</v>
+        <v>127</v>
+      </c>
+      <c r="C39" s="94" t="s">
+        <v>105</v>
       </c>
       <c r="D39" s="73"/>
       <c r="E39" s="73" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="F39" s="73" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="G39" s="73"/>
       <c r="H39" s="74"/>
     </row>
-    <row r="40" spans="1:8" ht="35" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="82"/>
+    <row r="40" spans="1:8" ht="32.25" thickBot="1">
+      <c r="A40" s="106"/>
       <c r="B40" s="59" t="s">
         <v>77</v>
       </c>
-      <c r="C40" s="112"/>
+      <c r="C40" s="92"/>
       <c r="D40" s="59"/>
       <c r="E40" s="59" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="F40" s="59" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="G40" s="75"/>
       <c r="H40" s="76"/>
     </row>
-    <row r="41" spans="1:8" ht="25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A41" s="83" t="s">
+    <row r="41" spans="1:8" ht="24.95" customHeight="1">
+      <c r="A41" s="107" t="s">
         <v>63</v>
       </c>
       <c r="B41" s="73" t="s">
         <v>14</v>
       </c>
-      <c r="C41" s="114" t="s">
+      <c r="C41" s="94" t="s">
         <v>24</v>
       </c>
       <c r="D41" s="73"/>
       <c r="E41" s="73" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="F41" s="73" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="G41" s="73"/>
       <c r="H41" s="74"/>
     </row>
-    <row r="42" spans="1:8" ht="24" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A42" s="84"/>
+    <row r="42" spans="1:8" ht="24" customHeight="1">
+      <c r="A42" s="108"/>
       <c r="B42" s="66" t="s">
         <v>15</v>
       </c>
-      <c r="C42" s="116" t="s">
-        <v>104</v>
+      <c r="C42" s="96" t="s">
+        <v>103</v>
       </c>
       <c r="D42" s="66"/>
       <c r="E42" s="66" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="F42" s="66" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="G42" s="66" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="H42" s="67"/>
     </row>
-    <row r="43" spans="1:8" ht="36" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A43" s="84"/>
+    <row r="43" spans="1:8" ht="36" customHeight="1">
+      <c r="A43" s="108"/>
       <c r="B43" s="57" t="s">
         <v>16</v>
       </c>
-      <c r="C43" s="111" t="s">
-        <v>108</v>
+      <c r="C43" s="91" t="s">
+        <v>107</v>
       </c>
       <c r="D43" s="57"/>
       <c r="E43" s="57" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="F43" s="57" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="G43" s="57" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="H43" s="58" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="44" spans="1:8" ht="24" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A44" s="84"/>
+        <v>106</v>
+      </c>
+    </row>
+    <row r="44" spans="1:8" ht="24" customHeight="1">
+      <c r="A44" s="108"/>
       <c r="B44" s="66" t="s">
-        <v>109</v>
-      </c>
-      <c r="C44" s="116" t="s">
+        <v>108</v>
+      </c>
+      <c r="C44" s="96" t="s">
         <v>22</v>
       </c>
       <c r="D44" s="66"/>
@@ -2506,12 +2506,12 @@
       </c>
       <c r="H44" s="67"/>
     </row>
-    <row r="45" spans="1:8" ht="33.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A45" s="84"/>
+    <row r="45" spans="1:8" ht="33.6" customHeight="1">
+      <c r="A45" s="108"/>
       <c r="B45" s="57" t="s">
         <v>19</v>
       </c>
-      <c r="C45" s="111" t="s">
+      <c r="C45" s="91" t="s">
         <v>21</v>
       </c>
       <c r="D45" s="57"/>
@@ -2519,87 +2519,87 @@
       <c r="F45" s="57"/>
       <c r="G45" s="57"/>
       <c r="H45" s="58" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="46" spans="1:8" ht="32" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A46" s="85"/>
+        <v>140</v>
+      </c>
+    </row>
+    <row r="46" spans="1:8" ht="32.1" customHeight="1" thickBot="1">
+      <c r="A46" s="109"/>
       <c r="B46" s="59" t="s">
+        <v>84</v>
+      </c>
+      <c r="C46" s="92"/>
+      <c r="D46" s="59" t="s">
         <v>85</v>
-      </c>
-      <c r="C46" s="112"/>
-      <c r="D46" s="59" t="s">
-        <v>86</v>
       </c>
       <c r="E46" s="75"/>
       <c r="F46" s="75"/>
       <c r="G46" s="75"/>
       <c r="H46" s="76"/>
     </row>
-    <row r="47" spans="1:8" ht="50" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A47" s="86" t="s">
+    <row r="47" spans="1:8" ht="50.1" customHeight="1">
+      <c r="A47" s="110" t="s">
         <v>64</v>
       </c>
       <c r="B47" s="73" t="s">
-        <v>128</v>
-      </c>
-      <c r="C47" s="114" t="s">
-        <v>106</v>
+        <v>127</v>
+      </c>
+      <c r="C47" s="94" t="s">
+        <v>105</v>
       </c>
       <c r="D47" s="73"/>
       <c r="E47" s="73" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="F47" s="73" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="G47" s="73" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="H47" s="74" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="48" spans="1:8" ht="24" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A48" s="86"/>
+    <row r="48" spans="1:8" ht="24" customHeight="1">
+      <c r="A48" s="110"/>
       <c r="B48" s="66" t="s">
-        <v>78</v>
-      </c>
-      <c r="C48" s="116"/>
+        <v>152</v>
+      </c>
+      <c r="C48" s="96"/>
       <c r="D48" s="66"/>
       <c r="E48" s="66"/>
       <c r="F48" s="66"/>
       <c r="G48" s="66" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="H48" s="67"/>
     </row>
-    <row r="49" spans="1:8" ht="34" x14ac:dyDescent="0.2">
-      <c r="A49" s="86"/>
+    <row r="49" spans="1:8" ht="31.5">
+      <c r="A49" s="110"/>
       <c r="B49" s="57" t="s">
         <v>77</v>
       </c>
-      <c r="C49" s="111"/>
+      <c r="C49" s="91"/>
       <c r="D49" s="57"/>
       <c r="E49" s="57" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="F49" s="57" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="G49" s="57" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="H49" s="58" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="50" spans="1:8" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A50" s="87"/>
+        <v>109</v>
+      </c>
+    </row>
+    <row r="50" spans="1:8" ht="24" customHeight="1" thickBot="1">
+      <c r="A50" s="111"/>
       <c r="B50" s="59" t="s">
-        <v>79</v>
-      </c>
-      <c r="C50" s="112"/>
+        <v>78</v>
+      </c>
+      <c r="C50" s="92"/>
       <c r="D50" s="59"/>
       <c r="E50" s="59" t="s">
         <v>4</v>
@@ -2612,16 +2612,16 @@
       </c>
       <c r="H50" s="60"/>
     </row>
-    <row r="51" spans="1:8" ht="35" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:8" ht="32.25" thickBot="1">
       <c r="A51" s="21" t="s">
+        <v>86</v>
+      </c>
+      <c r="B51" s="55" t="s">
         <v>87</v>
       </c>
-      <c r="B51" s="55" t="s">
+      <c r="C51" s="99"/>
+      <c r="D51" s="55" t="s">
         <v>88</v>
-      </c>
-      <c r="C51" s="119"/>
-      <c r="D51" s="55" t="s">
-        <v>89</v>
       </c>
       <c r="E51" s="55"/>
       <c r="F51" s="55"/>
@@ -2653,38 +2653,38 @@
   </sheetPr>
   <dimension ref="A1:E29"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <selection activeCell="D32" sqref="D32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="10.625" defaultRowHeight="15.75"/>
   <cols>
     <col min="1" max="1" width="22" customWidth="1"/>
     <col min="2" max="2" width="23" customWidth="1"/>
     <col min="3" max="3" width="25" customWidth="1"/>
-    <col min="4" max="4" width="56.1640625" customWidth="1"/>
-    <col min="5" max="5" width="46.6640625" customWidth="1"/>
-    <col min="10" max="10" width="11.33203125" customWidth="1"/>
+    <col min="4" max="4" width="56.125" customWidth="1"/>
+    <col min="5" max="5" width="46.625" customWidth="1"/>
+    <col min="10" max="10" width="11.375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="8" customFormat="1" ht="25" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" s="8" customFormat="1" ht="24" thickBot="1">
       <c r="A1" s="12" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B1" s="12" t="s">
         <v>1</v>
       </c>
       <c r="C1" s="12" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="D1" s="12" t="s">
         <v>49</v>
       </c>
       <c r="E1" s="12" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" ht="21" x14ac:dyDescent="0.25">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="21">
       <c r="A2" s="13" t="s">
         <v>47</v>
       </c>
@@ -2693,25 +2693,25 @@
       <c r="D2" s="9"/>
       <c r="E2" s="9"/>
     </row>
-    <row r="3" spans="1:5" ht="21" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" ht="21">
       <c r="A3" s="14"/>
       <c r="B3" s="10" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="C3" s="10"/>
       <c r="D3" s="10"/>
       <c r="E3" s="10"/>
     </row>
-    <row r="4" spans="1:5" ht="21" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" ht="21">
       <c r="A4" s="14"/>
       <c r="B4" s="10" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="C4" s="10"/>
       <c r="D4" s="10"/>
       <c r="E4" s="10"/>
     </row>
-    <row r="5" spans="1:5" ht="21" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" ht="21">
       <c r="A5" s="14"/>
       <c r="B5" s="10" t="s">
         <v>41</v>
@@ -2722,7 +2722,7 @@
       </c>
       <c r="E5" s="10"/>
     </row>
-    <row r="6" spans="1:5" ht="21" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" ht="21">
       <c r="A6" s="14"/>
       <c r="B6" s="10" t="s">
         <v>42</v>
@@ -2733,7 +2733,7 @@
       </c>
       <c r="E6" s="10"/>
     </row>
-    <row r="7" spans="1:5" ht="21" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" ht="21">
       <c r="A7" s="14"/>
       <c r="B7" s="10" t="s">
         <v>43</v>
@@ -2744,7 +2744,7 @@
       </c>
       <c r="E7" s="10"/>
     </row>
-    <row r="8" spans="1:5" ht="21" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" ht="21">
       <c r="A8" s="14"/>
       <c r="B8" s="10" t="s">
         <v>45</v>
@@ -2755,7 +2755,7 @@
       </c>
       <c r="E8" s="10"/>
     </row>
-    <row r="9" spans="1:5" ht="22" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:5" ht="21.75" thickBot="1">
       <c r="A9" s="15"/>
       <c r="B9" s="11" t="s">
         <v>38</v>
@@ -2766,7 +2766,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="10" spans="1:5" ht="21" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" ht="21">
       <c r="A10" s="13" t="s">
         <v>48</v>
       </c>
@@ -2775,29 +2775,29 @@
       <c r="D10" s="9"/>
       <c r="E10" s="9"/>
     </row>
-    <row r="11" spans="1:5" ht="21" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" ht="21">
       <c r="A11" s="14"/>
       <c r="B11" s="10" t="s">
         <v>50</v>
       </c>
       <c r="C11" s="10"/>
       <c r="D11" s="10" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="E11" s="10"/>
     </row>
-    <row r="12" spans="1:5" ht="21" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" ht="21">
       <c r="A12" s="14"/>
       <c r="B12" s="10" t="s">
         <v>51</v>
       </c>
       <c r="C12" s="10"/>
       <c r="D12" s="10" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="E12" s="10"/>
     </row>
-    <row r="13" spans="1:5" ht="21" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" ht="21">
       <c r="A13" s="14"/>
       <c r="B13" s="10" t="s">
         <v>52</v>
@@ -2806,18 +2806,18 @@
       <c r="D13" s="10"/>
       <c r="E13" s="10"/>
     </row>
-    <row r="14" spans="1:5" ht="22" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:5" ht="21.75" thickBot="1">
       <c r="A14" s="15"/>
       <c r="B14" s="11" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="C14" s="11"/>
       <c r="D14" s="11" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="E14" s="11"/>
     </row>
-    <row r="15" spans="1:5" ht="21" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" ht="21">
       <c r="A15" s="13" t="s">
         <v>53</v>
       </c>
@@ -2826,7 +2826,7 @@
       <c r="D15" s="9"/>
       <c r="E15" s="9"/>
     </row>
-    <row r="16" spans="1:5" ht="21" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" ht="21">
       <c r="A16" s="14"/>
       <c r="B16" s="10" t="s">
         <v>54</v>
@@ -2835,7 +2835,7 @@
       <c r="D16" s="10"/>
       <c r="E16" s="10"/>
     </row>
-    <row r="17" spans="1:5" ht="21" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" ht="21">
       <c r="A17" s="14"/>
       <c r="B17" s="10" t="s">
         <v>55</v>
@@ -2844,7 +2844,7 @@
       <c r="D17" s="10"/>
       <c r="E17" s="10"/>
     </row>
-    <row r="18" spans="1:5" ht="21" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" ht="21">
       <c r="A18" s="14"/>
       <c r="B18" s="10" t="s">
         <v>56</v>
@@ -2853,7 +2853,7 @@
       <c r="D18" s="10"/>
       <c r="E18" s="10"/>
     </row>
-    <row r="19" spans="1:5" ht="22" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:5" ht="21.75" thickBot="1">
       <c r="A19" s="15"/>
       <c r="B19" s="11" t="s">
         <v>57</v>
@@ -2862,59 +2862,59 @@
       <c r="D19" s="11"/>
       <c r="E19" s="11"/>
     </row>
-    <row r="20" spans="1:5" ht="21" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5" ht="21">
       <c r="A20" s="13" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B20" s="9"/>
       <c r="C20" s="9"/>
       <c r="D20" s="9"/>
       <c r="E20" s="9"/>
     </row>
-    <row r="21" spans="1:5" ht="21" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5" ht="21">
       <c r="A21" s="14"/>
       <c r="B21" s="10" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="C21" s="10"/>
       <c r="D21" s="10" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="E21" s="10"/>
     </row>
-    <row r="22" spans="1:5" ht="21" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:5" ht="21">
       <c r="A22" s="14"/>
       <c r="B22" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="C22" s="10"/>
       <c r="D22" s="10" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="E22" s="10"/>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:5">
       <c r="A23" s="4"/>
       <c r="B23" s="4"/>
       <c r="C23" s="4"/>
       <c r="D23" s="4"/>
       <c r="E23" s="4"/>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:5">
       <c r="A24" s="4"/>
       <c r="B24" s="4"/>
       <c r="C24" s="4"/>
       <c r="D24" s="4"/>
       <c r="E24" s="4"/>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:5">
       <c r="A25" s="7"/>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:5">
       <c r="A26" s="7"/>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="D29" s="123"/>
+    <row r="29" spans="1:5">
+      <c r="D29" s="103"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2933,13 +2933,13 @@
       <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2">
       <c r="A1" t="s">
-        <v>152</v>
-      </c>
-      <c r="B1" s="124">
+        <v>151</v>
+      </c>
+      <c r="B1" s="104">
         <v>44123</v>
       </c>
     </row>

</xml_diff>